<commit_message>
Sem 2 Major Update
Sem 2 Major Update
</commit_message>
<xml_diff>
--- a/Batch 2018-20/Sem 2/Notice Board.xlsx
+++ b/Batch 2018-20/Sem 2/Notice Board.xlsx
@@ -1,32 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Git\SIMSR-Results-Generator\Batch 2018-20\Sem 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8328E4FE-DCEB-4D16-AF57-3FD6E9CC840A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAC3D963-CFE6-430F-8E0D-1ED66E2738BC}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Notice Board" sheetId="1" r:id="rId1"/>
-    <sheet name="Top 5" sheetId="2" r:id="rId2"/>
   </sheets>
   <externalReferences>
+    <externalReference r:id="rId2"/>
     <externalReference r:id="rId3"/>
     <externalReference r:id="rId4"/>
-    <externalReference r:id="rId5"/>
   </externalReferences>
   <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="7">
   <si>
     <t>Name of Student</t>
   </si>
@@ -51,42 +50,12 @@
   <si>
     <t>Grade</t>
   </si>
-  <si>
-    <t>Top 5</t>
-  </si>
-  <si>
-    <t>Rank</t>
-  </si>
-  <si>
-    <t>Student Name</t>
-  </si>
-  <si>
-    <t>SGPI</t>
-  </si>
-  <si>
-    <t>Overall Grade</t>
-  </si>
-  <si>
-    <t>1st</t>
-  </si>
-  <si>
-    <t>2nd</t>
-  </si>
-  <si>
-    <t>3rd</t>
-  </si>
-  <si>
-    <t>4th</t>
-  </si>
-  <si>
-    <t>5th</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -121,28 +90,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="24"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="20"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="24"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -152,7 +99,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -285,110 +232,34 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
@@ -396,18 +267,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
@@ -420,30 +281,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1667,7 +1504,7 @@
             <v>70</v>
           </cell>
           <cell r="T3" t="str">
-            <v>A+</v>
+            <v>A</v>
           </cell>
           <cell r="U3" t="str">
             <v>8</v>
@@ -1867,7 +1704,7 @@
             <v>60</v>
           </cell>
           <cell r="T4" t="str">
-            <v>A</v>
+            <v>B</v>
           </cell>
           <cell r="U4" t="str">
             <v>6</v>
@@ -2067,7 +1904,7 @@
             <v>74</v>
           </cell>
           <cell r="T5" t="str">
-            <v>A+</v>
+            <v>A</v>
           </cell>
           <cell r="U5" t="str">
             <v>8</v>
@@ -2467,7 +2304,7 @@
             <v>69</v>
           </cell>
           <cell r="T7" t="str">
-            <v>A</v>
+            <v>B+</v>
           </cell>
           <cell r="U7" t="str">
             <v>7</v>
@@ -2667,7 +2504,7 @@
             <v>71</v>
           </cell>
           <cell r="T8" t="str">
-            <v>A+</v>
+            <v>A</v>
           </cell>
           <cell r="U8" t="str">
             <v>8</v>
@@ -2867,7 +2704,7 @@
             <v>71</v>
           </cell>
           <cell r="T9" t="str">
-            <v>A+</v>
+            <v>A</v>
           </cell>
           <cell r="U9" t="str">
             <v>8</v>
@@ -3267,7 +3104,7 @@
             <v>67</v>
           </cell>
           <cell r="T11" t="str">
-            <v>A</v>
+            <v>B+</v>
           </cell>
           <cell r="U11" t="str">
             <v>7</v>
@@ -3467,7 +3304,7 @@
             <v>69</v>
           </cell>
           <cell r="T12" t="str">
-            <v>A</v>
+            <v>B+</v>
           </cell>
           <cell r="U12" t="str">
             <v>7</v>
@@ -3667,7 +3504,7 @@
             <v>65</v>
           </cell>
           <cell r="T13" t="str">
-            <v>A</v>
+            <v>B+</v>
           </cell>
           <cell r="U13" t="str">
             <v>7</v>
@@ -3867,7 +3704,7 @@
             <v>70</v>
           </cell>
           <cell r="T14" t="str">
-            <v>A+</v>
+            <v>A</v>
           </cell>
           <cell r="U14" t="str">
             <v>8</v>
@@ -4067,7 +3904,7 @@
             <v>60</v>
           </cell>
           <cell r="T15" t="str">
-            <v>A</v>
+            <v>B</v>
           </cell>
           <cell r="U15" t="str">
             <v>6</v>
@@ -4267,7 +4104,7 @@
             <v>74</v>
           </cell>
           <cell r="T16" t="str">
-            <v>A+</v>
+            <v>A</v>
           </cell>
           <cell r="U16" t="str">
             <v>8</v>
@@ -4667,7 +4504,7 @@
             <v>69</v>
           </cell>
           <cell r="T18" t="str">
-            <v>A</v>
+            <v>B+</v>
           </cell>
           <cell r="U18" t="str">
             <v>7</v>
@@ -4867,7 +4704,7 @@
             <v>71</v>
           </cell>
           <cell r="T19" t="str">
-            <v>A+</v>
+            <v>A</v>
           </cell>
           <cell r="U19" t="str">
             <v>8</v>
@@ -5067,7 +4904,7 @@
             <v>71</v>
           </cell>
           <cell r="T20" t="str">
-            <v>A+</v>
+            <v>A</v>
           </cell>
           <cell r="U20" t="str">
             <v>8</v>
@@ -5467,7 +5304,7 @@
             <v>67</v>
           </cell>
           <cell r="T22" t="str">
-            <v>A</v>
+            <v>B+</v>
           </cell>
           <cell r="U22" t="str">
             <v>7</v>
@@ -5667,7 +5504,7 @@
             <v>69</v>
           </cell>
           <cell r="T23" t="str">
-            <v>A</v>
+            <v>B+</v>
           </cell>
           <cell r="U23" t="str">
             <v>7</v>
@@ -6067,7 +5904,7 @@
             <v>70</v>
           </cell>
           <cell r="T25" t="str">
-            <v>A+</v>
+            <v>A</v>
           </cell>
           <cell r="U25" t="str">
             <v>8</v>
@@ -6267,7 +6104,7 @@
             <v>60</v>
           </cell>
           <cell r="T26" t="str">
-            <v>A</v>
+            <v>B</v>
           </cell>
           <cell r="U26" t="str">
             <v>6</v>
@@ -6467,7 +6304,7 @@
             <v>74</v>
           </cell>
           <cell r="T27" t="str">
-            <v>A+</v>
+            <v>A</v>
           </cell>
           <cell r="U27" t="str">
             <v>8</v>
@@ -6867,7 +6704,7 @@
             <v>69</v>
           </cell>
           <cell r="T29" t="str">
-            <v>A</v>
+            <v>B+</v>
           </cell>
           <cell r="U29" t="str">
             <v>7</v>
@@ -7067,7 +6904,7 @@
             <v>71</v>
           </cell>
           <cell r="T30" t="str">
-            <v>A+</v>
+            <v>A</v>
           </cell>
           <cell r="U30" t="str">
             <v>8</v>
@@ -7267,7 +7104,7 @@
             <v>71</v>
           </cell>
           <cell r="T31" t="str">
-            <v>A+</v>
+            <v>A</v>
           </cell>
           <cell r="U31" t="str">
             <v>8</v>
@@ -7667,7 +7504,7 @@
             <v>67</v>
           </cell>
           <cell r="T33" t="str">
-            <v>A</v>
+            <v>B+</v>
           </cell>
           <cell r="U33" t="str">
             <v>7</v>
@@ -7867,7 +7704,7 @@
             <v>69</v>
           </cell>
           <cell r="T34" t="str">
-            <v>A</v>
+            <v>B+</v>
           </cell>
           <cell r="U34" t="str">
             <v>7</v>
@@ -8067,7 +7904,7 @@
             <v>65</v>
           </cell>
           <cell r="T35" t="str">
-            <v>A</v>
+            <v>B+</v>
           </cell>
           <cell r="U35" t="str">
             <v>7</v>
@@ -8267,7 +8104,7 @@
             <v>70</v>
           </cell>
           <cell r="T36" t="str">
-            <v>A+</v>
+            <v>A</v>
           </cell>
           <cell r="U36" t="str">
             <v>8</v>
@@ -8467,7 +8304,7 @@
             <v>60</v>
           </cell>
           <cell r="T37" t="str">
-            <v>A</v>
+            <v>B</v>
           </cell>
           <cell r="U37" t="str">
             <v>6</v>
@@ -8667,7 +8504,7 @@
             <v>74</v>
           </cell>
           <cell r="T38" t="str">
-            <v>A+</v>
+            <v>A</v>
           </cell>
           <cell r="U38" t="str">
             <v>8</v>
@@ -9067,7 +8904,7 @@
             <v>69</v>
           </cell>
           <cell r="T40" t="str">
-            <v>A</v>
+            <v>B+</v>
           </cell>
           <cell r="U40" t="str">
             <v>7</v>
@@ -9267,7 +9104,7 @@
             <v>71</v>
           </cell>
           <cell r="T41" t="str">
-            <v>A+</v>
+            <v>A</v>
           </cell>
           <cell r="U41" t="str">
             <v>8</v>
@@ -9467,7 +9304,7 @@
             <v>71</v>
           </cell>
           <cell r="T42" t="str">
-            <v>A+</v>
+            <v>A</v>
           </cell>
           <cell r="U42" t="str">
             <v>8</v>
@@ -9867,7 +9704,7 @@
             <v>67</v>
           </cell>
           <cell r="T44" t="str">
-            <v>A</v>
+            <v>B+</v>
           </cell>
           <cell r="U44" t="str">
             <v>7</v>
@@ -10267,7 +10104,7 @@
             <v>65</v>
           </cell>
           <cell r="T46" t="str">
-            <v>A</v>
+            <v>B+</v>
           </cell>
           <cell r="U46" t="str">
             <v>7</v>
@@ -10467,7 +10304,7 @@
             <v>70</v>
           </cell>
           <cell r="T47" t="str">
-            <v>A+</v>
+            <v>A</v>
           </cell>
           <cell r="U47" t="str">
             <v>8</v>
@@ -10667,7 +10504,7 @@
             <v>60</v>
           </cell>
           <cell r="T48" t="str">
-            <v>A</v>
+            <v>B</v>
           </cell>
           <cell r="U48" t="str">
             <v>6</v>
@@ -10867,7 +10704,7 @@
             <v>74</v>
           </cell>
           <cell r="T49" t="str">
-            <v>A+</v>
+            <v>A</v>
           </cell>
           <cell r="U49" t="str">
             <v>8</v>
@@ -11267,7 +11104,7 @@
             <v>69</v>
           </cell>
           <cell r="T51" t="str">
-            <v>A</v>
+            <v>B+</v>
           </cell>
           <cell r="U51" t="str">
             <v>7</v>
@@ -11467,7 +11304,7 @@
             <v>71</v>
           </cell>
           <cell r="T52" t="str">
-            <v>A+</v>
+            <v>A</v>
           </cell>
           <cell r="U52" t="str">
             <v>8</v>
@@ -11667,7 +11504,7 @@
             <v>71</v>
           </cell>
           <cell r="T53" t="str">
-            <v>A+</v>
+            <v>A</v>
           </cell>
           <cell r="U53" t="str">
             <v>8</v>
@@ -12067,7 +11904,7 @@
             <v>67</v>
           </cell>
           <cell r="T55" t="str">
-            <v>A</v>
+            <v>B+</v>
           </cell>
           <cell r="U55" t="str">
             <v>7</v>
@@ -12267,7 +12104,7 @@
             <v>69</v>
           </cell>
           <cell r="T56" t="str">
-            <v>A</v>
+            <v>B+</v>
           </cell>
           <cell r="U56" t="str">
             <v>7</v>
@@ -12467,7 +12304,7 @@
             <v>65</v>
           </cell>
           <cell r="T57" t="str">
-            <v>A</v>
+            <v>B+</v>
           </cell>
           <cell r="U57" t="str">
             <v>7</v>
@@ -12667,7 +12504,7 @@
             <v>70</v>
           </cell>
           <cell r="T58" t="str">
-            <v>A+</v>
+            <v>A</v>
           </cell>
           <cell r="U58" t="str">
             <v>8</v>
@@ -12867,7 +12704,7 @@
             <v>60</v>
           </cell>
           <cell r="T59" t="str">
-            <v>A</v>
+            <v>B</v>
           </cell>
           <cell r="U59" t="str">
             <v>6</v>
@@ -13067,7 +12904,7 @@
             <v>74</v>
           </cell>
           <cell r="T60" t="str">
-            <v>A+</v>
+            <v>A</v>
           </cell>
           <cell r="U60" t="str">
             <v>8</v>
@@ -13467,7 +13304,7 @@
             <v>69</v>
           </cell>
           <cell r="T62" t="str">
-            <v>A</v>
+            <v>B+</v>
           </cell>
           <cell r="U62" t="str">
             <v>7</v>
@@ -13667,7 +13504,7 @@
             <v>71</v>
           </cell>
           <cell r="T63" t="str">
-            <v>A+</v>
+            <v>A</v>
           </cell>
           <cell r="U63" t="str">
             <v>8</v>
@@ -13867,7 +13704,7 @@
             <v>71</v>
           </cell>
           <cell r="T64" t="str">
-            <v>A+</v>
+            <v>A</v>
           </cell>
           <cell r="U64" t="str">
             <v>8</v>
@@ -14267,7 +14104,7 @@
             <v>67</v>
           </cell>
           <cell r="T66" t="str">
-            <v>A</v>
+            <v>B+</v>
           </cell>
           <cell r="U66" t="str">
             <v>7</v>
@@ -14467,7 +14304,7 @@
             <v>69</v>
           </cell>
           <cell r="T67" t="str">
-            <v>A</v>
+            <v>B+</v>
           </cell>
           <cell r="U67" t="str">
             <v>7</v>
@@ -14667,7 +14504,7 @@
             <v>65</v>
           </cell>
           <cell r="T68" t="str">
-            <v>A</v>
+            <v>B+</v>
           </cell>
           <cell r="U68" t="str">
             <v>7</v>
@@ -14867,7 +14704,7 @@
             <v>70</v>
           </cell>
           <cell r="T69" t="str">
-            <v>A+</v>
+            <v>A</v>
           </cell>
           <cell r="U69" t="str">
             <v>8</v>
@@ -15067,7 +14904,7 @@
             <v>60</v>
           </cell>
           <cell r="T70" t="str">
-            <v>A</v>
+            <v>B</v>
           </cell>
           <cell r="U70" t="str">
             <v>6</v>
@@ -15267,7 +15104,7 @@
             <v>74</v>
           </cell>
           <cell r="T71" t="str">
-            <v>A+</v>
+            <v>A</v>
           </cell>
           <cell r="U71" t="str">
             <v>8</v>
@@ -15667,7 +15504,7 @@
             <v>69</v>
           </cell>
           <cell r="T73" t="str">
-            <v>A</v>
+            <v>B+</v>
           </cell>
           <cell r="U73" t="str">
             <v>7</v>
@@ -15867,7 +15704,7 @@
             <v>71</v>
           </cell>
           <cell r="T74" t="str">
-            <v>A+</v>
+            <v>A</v>
           </cell>
           <cell r="U74" t="str">
             <v>8</v>
@@ -16067,7 +15904,7 @@
             <v>71</v>
           </cell>
           <cell r="T75" t="str">
-            <v>A+</v>
+            <v>A</v>
           </cell>
           <cell r="U75" t="str">
             <v>8</v>
@@ -16467,7 +16304,7 @@
             <v>67</v>
           </cell>
           <cell r="T77" t="str">
-            <v>A</v>
+            <v>B+</v>
           </cell>
           <cell r="U77" t="str">
             <v>7</v>
@@ -16667,7 +16504,7 @@
             <v>69</v>
           </cell>
           <cell r="T78" t="str">
-            <v>A</v>
+            <v>B+</v>
           </cell>
           <cell r="U78" t="str">
             <v>7</v>
@@ -16867,7 +16704,7 @@
             <v>65</v>
           </cell>
           <cell r="T79" t="str">
-            <v>A</v>
+            <v>B+</v>
           </cell>
           <cell r="U79" t="str">
             <v>7</v>
@@ -17067,7 +16904,7 @@
             <v>70</v>
           </cell>
           <cell r="T80" t="str">
-            <v>A+</v>
+            <v>A</v>
           </cell>
           <cell r="U80" t="str">
             <v>8</v>
@@ -17267,7 +17104,7 @@
             <v>60</v>
           </cell>
           <cell r="T81" t="str">
-            <v>A</v>
+            <v>B</v>
           </cell>
           <cell r="U81" t="str">
             <v>6</v>
@@ -17467,7 +17304,7 @@
             <v>74</v>
           </cell>
           <cell r="T82" t="str">
-            <v>A+</v>
+            <v>A</v>
           </cell>
           <cell r="U82" t="str">
             <v>8</v>
@@ -17867,7 +17704,7 @@
             <v>69</v>
           </cell>
           <cell r="T84" t="str">
-            <v>A</v>
+            <v>B+</v>
           </cell>
           <cell r="U84" t="str">
             <v>7</v>
@@ -18067,7 +17904,7 @@
             <v>71</v>
           </cell>
           <cell r="T85" t="str">
-            <v>A+</v>
+            <v>A</v>
           </cell>
           <cell r="U85" t="str">
             <v>8</v>
@@ -18267,7 +18104,7 @@
             <v>71</v>
           </cell>
           <cell r="T86" t="str">
-            <v>A+</v>
+            <v>A</v>
           </cell>
           <cell r="U86" t="str">
             <v>8</v>
@@ -18667,7 +18504,7 @@
             <v>67</v>
           </cell>
           <cell r="T88" t="str">
-            <v>A</v>
+            <v>B+</v>
           </cell>
           <cell r="U88" t="str">
             <v>7</v>
@@ -18867,7 +18704,7 @@
             <v>69</v>
           </cell>
           <cell r="T89" t="str">
-            <v>A</v>
+            <v>B+</v>
           </cell>
           <cell r="U89" t="str">
             <v>7</v>
@@ -19067,7 +18904,7 @@
             <v>65</v>
           </cell>
           <cell r="T90" t="str">
-            <v>A</v>
+            <v>B+</v>
           </cell>
           <cell r="U90" t="str">
             <v>7</v>
@@ -19267,7 +19104,7 @@
             <v>70</v>
           </cell>
           <cell r="T91" t="str">
-            <v>A+</v>
+            <v>A</v>
           </cell>
           <cell r="U91" t="str">
             <v>8</v>
@@ -19467,7 +19304,7 @@
             <v>60</v>
           </cell>
           <cell r="T92" t="str">
-            <v>A</v>
+            <v>B</v>
           </cell>
           <cell r="U92" t="str">
             <v>6</v>
@@ -19667,7 +19504,7 @@
             <v>74</v>
           </cell>
           <cell r="T93" t="str">
-            <v>A+</v>
+            <v>A</v>
           </cell>
           <cell r="U93" t="str">
             <v>8</v>
@@ -20067,7 +19904,7 @@
             <v>69</v>
           </cell>
           <cell r="T95" t="str">
-            <v>A</v>
+            <v>B+</v>
           </cell>
           <cell r="U95" t="str">
             <v>7</v>
@@ -20267,7 +20104,7 @@
             <v>71</v>
           </cell>
           <cell r="T96" t="str">
-            <v>A+</v>
+            <v>A</v>
           </cell>
           <cell r="U96" t="str">
             <v>8</v>
@@ -20467,7 +20304,7 @@
             <v>71</v>
           </cell>
           <cell r="T97" t="str">
-            <v>A+</v>
+            <v>A</v>
           </cell>
           <cell r="U97" t="str">
             <v>8</v>
@@ -20867,7 +20704,7 @@
             <v>67</v>
           </cell>
           <cell r="T99" t="str">
-            <v>A</v>
+            <v>B+</v>
           </cell>
           <cell r="U99" t="str">
             <v>7</v>
@@ -21067,7 +20904,7 @@
             <v>69</v>
           </cell>
           <cell r="T100" t="str">
-            <v>A</v>
+            <v>B+</v>
           </cell>
           <cell r="U100" t="str">
             <v>7</v>
@@ -21267,7 +21104,7 @@
             <v>65</v>
           </cell>
           <cell r="T101" t="str">
-            <v>A</v>
+            <v>B+</v>
           </cell>
           <cell r="U101" t="str">
             <v>7</v>
@@ -21467,7 +21304,7 @@
             <v>70</v>
           </cell>
           <cell r="T102" t="str">
-            <v>A+</v>
+            <v>A</v>
           </cell>
           <cell r="U102" t="str">
             <v>8</v>
@@ -21667,7 +21504,7 @@
             <v>60</v>
           </cell>
           <cell r="T103" t="str">
-            <v>A</v>
+            <v>B</v>
           </cell>
           <cell r="U103" t="str">
             <v>6</v>
@@ -21867,7 +21704,7 @@
             <v>74</v>
           </cell>
           <cell r="T104" t="str">
-            <v>A+</v>
+            <v>A</v>
           </cell>
           <cell r="U104" t="str">
             <v>8</v>
@@ -22267,7 +22104,7 @@
             <v>69</v>
           </cell>
           <cell r="T106" t="str">
-            <v>A</v>
+            <v>B+</v>
           </cell>
           <cell r="U106" t="str">
             <v>7</v>
@@ -22467,7 +22304,7 @@
             <v>71</v>
           </cell>
           <cell r="T107" t="str">
-            <v>A+</v>
+            <v>A</v>
           </cell>
           <cell r="U107" t="str">
             <v>8</v>
@@ -22667,7 +22504,7 @@
             <v>71</v>
           </cell>
           <cell r="T108" t="str">
-            <v>A+</v>
+            <v>A</v>
           </cell>
           <cell r="U108" t="str">
             <v>8</v>
@@ -23067,7 +22904,7 @@
             <v>67</v>
           </cell>
           <cell r="T110" t="str">
-            <v>A</v>
+            <v>B+</v>
           </cell>
           <cell r="U110" t="str">
             <v>7</v>
@@ -23267,7 +23104,7 @@
             <v>69</v>
           </cell>
           <cell r="T111" t="str">
-            <v>A</v>
+            <v>B+</v>
           </cell>
           <cell r="U111" t="str">
             <v>7</v>
@@ -23467,7 +23304,7 @@
             <v>65</v>
           </cell>
           <cell r="T112" t="str">
-            <v>A</v>
+            <v>B+</v>
           </cell>
           <cell r="U112" t="str">
             <v>7</v>
@@ -23667,7 +23504,7 @@
             <v>70</v>
           </cell>
           <cell r="T113" t="str">
-            <v>A+</v>
+            <v>A</v>
           </cell>
           <cell r="U113" t="str">
             <v>8</v>
@@ -23867,7 +23704,7 @@
             <v>60</v>
           </cell>
           <cell r="T114" t="str">
-            <v>A</v>
+            <v>B</v>
           </cell>
           <cell r="U114" t="str">
             <v>6</v>
@@ -24067,7 +23904,7 @@
             <v>74</v>
           </cell>
           <cell r="T115" t="str">
-            <v>A+</v>
+            <v>A</v>
           </cell>
           <cell r="U115" t="str">
             <v>8</v>
@@ -24467,7 +24304,7 @@
             <v>69</v>
           </cell>
           <cell r="T117" t="str">
-            <v>A</v>
+            <v>B+</v>
           </cell>
           <cell r="U117" t="str">
             <v>7</v>
@@ -24667,7 +24504,7 @@
             <v>71</v>
           </cell>
           <cell r="T118" t="str">
-            <v>A+</v>
+            <v>A</v>
           </cell>
           <cell r="U118" t="str">
             <v>8</v>
@@ -24867,7 +24704,7 @@
             <v>71</v>
           </cell>
           <cell r="T119" t="str">
-            <v>A+</v>
+            <v>A</v>
           </cell>
           <cell r="U119" t="str">
             <v>8</v>
@@ -25267,7 +25104,7 @@
             <v>67</v>
           </cell>
           <cell r="T121" t="str">
-            <v>A</v>
+            <v>B+</v>
           </cell>
           <cell r="U121" t="str">
             <v>7</v>
@@ -28529,46 +28366,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="1" customFormat="1" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="12" t="str">
+      <c r="B1" s="13"/>
+      <c r="C1" s="10" t="str">
         <f>'[1]Subjects List'!$C$4</f>
         <v>Perspective Management</v>
       </c>
-      <c r="D1" s="10" t="str">
+      <c r="D1" s="9" t="str">
         <f>'[1]Subjects List'!$C$5</f>
         <v>Financial Accounting</v>
       </c>
-      <c r="E1" s="12" t="str">
+      <c r="E1" s="10" t="str">
         <f>'[1]Subjects List'!$C$6</f>
         <v>Business Statistics</v>
       </c>
-      <c r="F1" s="12" t="str">
+      <c r="F1" s="10" t="str">
         <f>'[1]Subjects List'!$C$7</f>
         <v>Operations Management</v>
       </c>
-      <c r="G1" s="12" t="str">
+      <c r="G1" s="10" t="str">
         <f>'[1]Subjects List'!$C$8</f>
         <v>Managerial Economics</v>
       </c>
-      <c r="H1" s="11" t="str">
+      <c r="H1" s="9" t="str">
         <f>'[1]Subjects List'!$C$9</f>
         <v>Effective and Management Communication</v>
       </c>
-      <c r="I1" s="11" t="str">
+      <c r="I1" s="9" t="str">
         <f>'[1]Subjects List'!$C$10</f>
         <v>Negotiation and Selling Skills</v>
       </c>
-      <c r="J1" s="11" t="str">
+      <c r="J1" s="9" t="str">
         <f>'[1]Subjects List'!$C$11</f>
         <v>Organisational Behaviour</v>
       </c>
-      <c r="K1" s="20" t="s">
+      <c r="K1" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="L1" s="21"/>
+      <c r="L1" s="15"/>
     </row>
     <row r="2" spans="1:12" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
@@ -28601,15 +28438,15 @@
       <c r="J2" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="K2" s="9" t="s">
+      <c r="K2" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="L2" s="9" t="s">
+      <c r="L2" s="8" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="13" t="str">
+      <c r="A3" s="11" t="str">
         <f>[2]Sheet1!$A2</f>
         <v>MMS18-20/001</v>
       </c>
@@ -28627,7 +28464,7 @@
       </c>
       <c r="E3" s="6" t="str">
         <f>'[3]Subject Marks'!$T3</f>
-        <v>A+</v>
+        <v>A</v>
       </c>
       <c r="F3" s="6" t="str">
         <f>'[3]Subject Marks'!$AA3</f>
@@ -28659,7 +28496,7 @@
       </c>
     </row>
     <row r="4" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="13" t="str">
+      <c r="A4" s="11" t="str">
         <f>[2]Sheet1!$A3</f>
         <v>MMS18-20/002</v>
       </c>
@@ -28677,7 +28514,7 @@
       </c>
       <c r="E4" s="6" t="str">
         <f>'[3]Subject Marks'!$T4</f>
-        <v>A</v>
+        <v>B</v>
       </c>
       <c r="F4" s="6" t="str">
         <f>'[3]Subject Marks'!$AA4</f>
@@ -28709,7 +28546,7 @@
       </c>
     </row>
     <row r="5" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="13" t="str">
+      <c r="A5" s="11" t="str">
         <f>[2]Sheet1!$A4</f>
         <v>MMS18-20/003</v>
       </c>
@@ -28727,7 +28564,7 @@
       </c>
       <c r="E5" s="6" t="str">
         <f>'[3]Subject Marks'!$T5</f>
-        <v>A+</v>
+        <v>A</v>
       </c>
       <c r="F5" s="6" t="str">
         <f>'[3]Subject Marks'!$AA5</f>
@@ -28759,7 +28596,7 @@
       </c>
     </row>
     <row r="6" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="13" t="str">
+      <c r="A6" s="11" t="str">
         <f>[2]Sheet1!$A5</f>
         <v>MMS18-20/004</v>
       </c>
@@ -28809,7 +28646,7 @@
       </c>
     </row>
     <row r="7" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="13" t="str">
+      <c r="A7" s="11" t="str">
         <f>[2]Sheet1!$A6</f>
         <v>MMS18-20/005</v>
       </c>
@@ -28827,7 +28664,7 @@
       </c>
       <c r="E7" s="6" t="str">
         <f>'[3]Subject Marks'!$T7</f>
-        <v>A</v>
+        <v>B+</v>
       </c>
       <c r="F7" s="6" t="str">
         <f>'[3]Subject Marks'!$AA7</f>
@@ -28859,7 +28696,7 @@
       </c>
     </row>
     <row r="8" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="13" t="str">
+      <c r="A8" s="11" t="str">
         <f>[2]Sheet1!$A7</f>
         <v>MMS18-20/006</v>
       </c>
@@ -28877,7 +28714,7 @@
       </c>
       <c r="E8" s="6" t="str">
         <f>'[3]Subject Marks'!$T8</f>
-        <v>A+</v>
+        <v>A</v>
       </c>
       <c r="F8" s="6" t="str">
         <f>'[3]Subject Marks'!$AA8</f>
@@ -28909,7 +28746,7 @@
       </c>
     </row>
     <row r="9" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="13" t="str">
+      <c r="A9" s="11" t="str">
         <f>[2]Sheet1!$A8</f>
         <v>MMS18-20/007</v>
       </c>
@@ -28927,7 +28764,7 @@
       </c>
       <c r="E9" s="6" t="str">
         <f>'[3]Subject Marks'!$T9</f>
-        <v>A+</v>
+        <v>A</v>
       </c>
       <c r="F9" s="6" t="str">
         <f>'[3]Subject Marks'!$AA9</f>
@@ -28959,7 +28796,7 @@
       </c>
     </row>
     <row r="10" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="13" t="str">
+      <c r="A10" s="11" t="str">
         <f>[2]Sheet1!$A9</f>
         <v>MMS18-20/008</v>
       </c>
@@ -29009,7 +28846,7 @@
       </c>
     </row>
     <row r="11" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="13" t="str">
+      <c r="A11" s="11" t="str">
         <f>[2]Sheet1!$A10</f>
         <v>MMS18-20/009</v>
       </c>
@@ -29027,7 +28864,7 @@
       </c>
       <c r="E11" s="6" t="str">
         <f>'[3]Subject Marks'!$T11</f>
-        <v>A</v>
+        <v>B+</v>
       </c>
       <c r="F11" s="6" t="str">
         <f>'[3]Subject Marks'!$AA11</f>
@@ -29059,7 +28896,7 @@
       </c>
     </row>
     <row r="12" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="13" t="str">
+      <c r="A12" s="11" t="str">
         <f>[2]Sheet1!$A11</f>
         <v>MMS18-20/010</v>
       </c>
@@ -29077,7 +28914,7 @@
       </c>
       <c r="E12" s="6" t="str">
         <f>'[3]Subject Marks'!$T12</f>
-        <v>A</v>
+        <v>B+</v>
       </c>
       <c r="F12" s="6" t="str">
         <f>'[3]Subject Marks'!$AA12</f>
@@ -29109,7 +28946,7 @@
       </c>
     </row>
     <row r="13" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="13" t="str">
+      <c r="A13" s="11" t="str">
         <f>[2]Sheet1!$A12</f>
         <v>MMS18-20/011</v>
       </c>
@@ -29127,7 +28964,7 @@
       </c>
       <c r="E13" s="6" t="str">
         <f>'[3]Subject Marks'!$T13</f>
-        <v>A</v>
+        <v>B+</v>
       </c>
       <c r="F13" s="6" t="str">
         <f>'[3]Subject Marks'!$AA13</f>
@@ -29159,7 +28996,7 @@
       </c>
     </row>
     <row r="14" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="13" t="str">
+      <c r="A14" s="11" t="str">
         <f>[2]Sheet1!$A13</f>
         <v>MMS18-20/012</v>
       </c>
@@ -29177,7 +29014,7 @@
       </c>
       <c r="E14" s="6" t="str">
         <f>'[3]Subject Marks'!$T14</f>
-        <v>A+</v>
+        <v>A</v>
       </c>
       <c r="F14" s="6" t="str">
         <f>'[3]Subject Marks'!$AA14</f>
@@ -29209,7 +29046,7 @@
       </c>
     </row>
     <row r="15" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="13" t="str">
+      <c r="A15" s="11" t="str">
         <f>[2]Sheet1!$A14</f>
         <v>MMS18-20/013</v>
       </c>
@@ -29227,7 +29064,7 @@
       </c>
       <c r="E15" s="6" t="str">
         <f>'[3]Subject Marks'!$T15</f>
-        <v>A</v>
+        <v>B</v>
       </c>
       <c r="F15" s="6" t="str">
         <f>'[3]Subject Marks'!$AA15</f>
@@ -29259,7 +29096,7 @@
       </c>
     </row>
     <row r="16" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="13" t="str">
+      <c r="A16" s="11" t="str">
         <f>[2]Sheet1!$A15</f>
         <v>MMS18-20/014</v>
       </c>
@@ -29277,7 +29114,7 @@
       </c>
       <c r="E16" s="6" t="str">
         <f>'[3]Subject Marks'!$T16</f>
-        <v>A+</v>
+        <v>A</v>
       </c>
       <c r="F16" s="6" t="str">
         <f>'[3]Subject Marks'!$AA16</f>
@@ -29309,7 +29146,7 @@
       </c>
     </row>
     <row r="17" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="13" t="str">
+      <c r="A17" s="11" t="str">
         <f>[2]Sheet1!$A16</f>
         <v>MMS18-20/015</v>
       </c>
@@ -29359,7 +29196,7 @@
       </c>
     </row>
     <row r="18" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="13" t="str">
+      <c r="A18" s="11" t="str">
         <f>[2]Sheet1!$A17</f>
         <v>MMS18-20/016</v>
       </c>
@@ -29377,7 +29214,7 @@
       </c>
       <c r="E18" s="6" t="str">
         <f>'[3]Subject Marks'!$T18</f>
-        <v>A</v>
+        <v>B+</v>
       </c>
       <c r="F18" s="6" t="str">
         <f>'[3]Subject Marks'!$AA18</f>
@@ -29409,7 +29246,7 @@
       </c>
     </row>
     <row r="19" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="13" t="str">
+      <c r="A19" s="11" t="str">
         <f>[2]Sheet1!$A18</f>
         <v>MMS18-20/017</v>
       </c>
@@ -29427,7 +29264,7 @@
       </c>
       <c r="E19" s="6" t="str">
         <f>'[3]Subject Marks'!$T19</f>
-        <v>A+</v>
+        <v>A</v>
       </c>
       <c r="F19" s="6" t="str">
         <f>'[3]Subject Marks'!$AA19</f>
@@ -29459,7 +29296,7 @@
       </c>
     </row>
     <row r="20" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="13" t="str">
+      <c r="A20" s="11" t="str">
         <f>[2]Sheet1!$A19</f>
         <v>MMS18-20/018</v>
       </c>
@@ -29477,7 +29314,7 @@
       </c>
       <c r="E20" s="6" t="str">
         <f>'[3]Subject Marks'!$T20</f>
-        <v>A+</v>
+        <v>A</v>
       </c>
       <c r="F20" s="6" t="str">
         <f>'[3]Subject Marks'!$AA20</f>
@@ -29509,7 +29346,7 @@
       </c>
     </row>
     <row r="21" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="13" t="str">
+      <c r="A21" s="11" t="str">
         <f>[2]Sheet1!$A20</f>
         <v>MMS18-20/019</v>
       </c>
@@ -29559,7 +29396,7 @@
       </c>
     </row>
     <row r="22" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="13" t="str">
+      <c r="A22" s="11" t="str">
         <f>[2]Sheet1!$A21</f>
         <v>MMS18-20/020</v>
       </c>
@@ -29577,7 +29414,7 @@
       </c>
       <c r="E22" s="6" t="str">
         <f>'[3]Subject Marks'!$T22</f>
-        <v>A</v>
+        <v>B+</v>
       </c>
       <c r="F22" s="6" t="str">
         <f>'[3]Subject Marks'!$AA22</f>
@@ -29609,7 +29446,7 @@
       </c>
     </row>
     <row r="23" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="13" t="str">
+      <c r="A23" s="11" t="str">
         <f>[2]Sheet1!$A22</f>
         <v>MMS18-20/021</v>
       </c>
@@ -29627,7 +29464,7 @@
       </c>
       <c r="E23" s="6" t="str">
         <f>'[3]Subject Marks'!$T23</f>
-        <v>A</v>
+        <v>B+</v>
       </c>
       <c r="F23" s="6" t="str">
         <f>'[3]Subject Marks'!$AA23</f>
@@ -29659,7 +29496,7 @@
       </c>
     </row>
     <row r="24" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="13" t="str">
+      <c r="A24" s="11" t="str">
         <f>[2]Sheet1!$A23</f>
         <v>MMS18-20/022</v>
       </c>
@@ -29709,7 +29546,7 @@
       </c>
     </row>
     <row r="25" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="13" t="str">
+      <c r="A25" s="11" t="str">
         <f>[2]Sheet1!$A24</f>
         <v>MMS18-20/023</v>
       </c>
@@ -29727,7 +29564,7 @@
       </c>
       <c r="E25" s="6" t="str">
         <f>'[3]Subject Marks'!$T25</f>
-        <v>A+</v>
+        <v>A</v>
       </c>
       <c r="F25" s="6" t="str">
         <f>'[3]Subject Marks'!$AA25</f>
@@ -29759,7 +29596,7 @@
       </c>
     </row>
     <row r="26" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="13" t="str">
+      <c r="A26" s="11" t="str">
         <f>[2]Sheet1!$A25</f>
         <v>MMS18-20/024</v>
       </c>
@@ -29777,7 +29614,7 @@
       </c>
       <c r="E26" s="6" t="str">
         <f>'[3]Subject Marks'!$T26</f>
-        <v>A</v>
+        <v>B</v>
       </c>
       <c r="F26" s="6" t="str">
         <f>'[3]Subject Marks'!$AA26</f>
@@ -29809,7 +29646,7 @@
       </c>
     </row>
     <row r="27" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A27" s="13" t="str">
+      <c r="A27" s="11" t="str">
         <f>[2]Sheet1!$A26</f>
         <v>MMS18-20/025</v>
       </c>
@@ -29827,7 +29664,7 @@
       </c>
       <c r="E27" s="6" t="str">
         <f>'[3]Subject Marks'!$T27</f>
-        <v>A+</v>
+        <v>A</v>
       </c>
       <c r="F27" s="6" t="str">
         <f>'[3]Subject Marks'!$AA27</f>
@@ -29859,7 +29696,7 @@
       </c>
     </row>
     <row r="28" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A28" s="13" t="str">
+      <c r="A28" s="11" t="str">
         <f>[2]Sheet1!$A27</f>
         <v>MMS18-20/026</v>
       </c>
@@ -29909,7 +29746,7 @@
       </c>
     </row>
     <row r="29" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A29" s="13" t="str">
+      <c r="A29" s="11" t="str">
         <f>[2]Sheet1!$A28</f>
         <v>MMS18-20/027</v>
       </c>
@@ -29927,7 +29764,7 @@
       </c>
       <c r="E29" s="6" t="str">
         <f>'[3]Subject Marks'!$T29</f>
-        <v>A</v>
+        <v>B+</v>
       </c>
       <c r="F29" s="6" t="str">
         <f>'[3]Subject Marks'!$AA29</f>
@@ -29959,7 +29796,7 @@
       </c>
     </row>
     <row r="30" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A30" s="13" t="str">
+      <c r="A30" s="11" t="str">
         <f>[2]Sheet1!$A29</f>
         <v>MMS18-20/028</v>
       </c>
@@ -29977,7 +29814,7 @@
       </c>
       <c r="E30" s="6" t="str">
         <f>'[3]Subject Marks'!$T30</f>
-        <v>A+</v>
+        <v>A</v>
       </c>
       <c r="F30" s="6" t="str">
         <f>'[3]Subject Marks'!$AA30</f>
@@ -30009,7 +29846,7 @@
       </c>
     </row>
     <row r="31" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A31" s="13" t="str">
+      <c r="A31" s="11" t="str">
         <f>[2]Sheet1!$A30</f>
         <v>MMS18-20/029</v>
       </c>
@@ -30027,7 +29864,7 @@
       </c>
       <c r="E31" s="6" t="str">
         <f>'[3]Subject Marks'!$T31</f>
-        <v>A+</v>
+        <v>A</v>
       </c>
       <c r="F31" s="6" t="str">
         <f>'[3]Subject Marks'!$AA31</f>
@@ -30059,7 +29896,7 @@
       </c>
     </row>
     <row r="32" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A32" s="13" t="str">
+      <c r="A32" s="11" t="str">
         <f>[2]Sheet1!$A31</f>
         <v>MMS18-20/030</v>
       </c>
@@ -30109,7 +29946,7 @@
       </c>
     </row>
     <row r="33" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A33" s="13" t="str">
+      <c r="A33" s="11" t="str">
         <f>[2]Sheet1!$A32</f>
         <v>MMS18-20/031</v>
       </c>
@@ -30127,7 +29964,7 @@
       </c>
       <c r="E33" s="6" t="str">
         <f>'[3]Subject Marks'!$T33</f>
-        <v>A</v>
+        <v>B+</v>
       </c>
       <c r="F33" s="6" t="str">
         <f>'[3]Subject Marks'!$AA33</f>
@@ -30159,7 +29996,7 @@
       </c>
     </row>
     <row r="34" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A34" s="13" t="str">
+      <c r="A34" s="11" t="str">
         <f>[2]Sheet1!$A33</f>
         <v>MMS18-20/032</v>
       </c>
@@ -30177,7 +30014,7 @@
       </c>
       <c r="E34" s="6" t="str">
         <f>'[3]Subject Marks'!$T34</f>
-        <v>A</v>
+        <v>B+</v>
       </c>
       <c r="F34" s="6" t="str">
         <f>'[3]Subject Marks'!$AA34</f>
@@ -30209,7 +30046,7 @@
       </c>
     </row>
     <row r="35" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A35" s="13" t="str">
+      <c r="A35" s="11" t="str">
         <f>[2]Sheet1!$A34</f>
         <v>MMS18-20/033</v>
       </c>
@@ -30227,7 +30064,7 @@
       </c>
       <c r="E35" s="6" t="str">
         <f>'[3]Subject Marks'!$T35</f>
-        <v>A</v>
+        <v>B+</v>
       </c>
       <c r="F35" s="6" t="str">
         <f>'[3]Subject Marks'!$AA35</f>
@@ -30259,7 +30096,7 @@
       </c>
     </row>
     <row r="36" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A36" s="13" t="str">
+      <c r="A36" s="11" t="str">
         <f>[2]Sheet1!$A35</f>
         <v>MMS18-20/034</v>
       </c>
@@ -30277,7 +30114,7 @@
       </c>
       <c r="E36" s="6" t="str">
         <f>'[3]Subject Marks'!$T36</f>
-        <v>A+</v>
+        <v>A</v>
       </c>
       <c r="F36" s="6" t="str">
         <f>'[3]Subject Marks'!$AA36</f>
@@ -30309,7 +30146,7 @@
       </c>
     </row>
     <row r="37" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A37" s="13" t="str">
+      <c r="A37" s="11" t="str">
         <f>[2]Sheet1!$A36</f>
         <v>MMS18-20/035</v>
       </c>
@@ -30327,7 +30164,7 @@
       </c>
       <c r="E37" s="6" t="str">
         <f>'[3]Subject Marks'!$T37</f>
-        <v>A</v>
+        <v>B</v>
       </c>
       <c r="F37" s="6" t="str">
         <f>'[3]Subject Marks'!$AA37</f>
@@ -30359,7 +30196,7 @@
       </c>
     </row>
     <row r="38" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A38" s="13" t="str">
+      <c r="A38" s="11" t="str">
         <f>[2]Sheet1!$A37</f>
         <v>MMS18-20/036</v>
       </c>
@@ -30377,7 +30214,7 @@
       </c>
       <c r="E38" s="6" t="str">
         <f>'[3]Subject Marks'!$T38</f>
-        <v>A+</v>
+        <v>A</v>
       </c>
       <c r="F38" s="6" t="str">
         <f>'[3]Subject Marks'!$AA38</f>
@@ -30409,7 +30246,7 @@
       </c>
     </row>
     <row r="39" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A39" s="13" t="str">
+      <c r="A39" s="11" t="str">
         <f>[2]Sheet1!$A38</f>
         <v>MMS18-20/037</v>
       </c>
@@ -30459,7 +30296,7 @@
       </c>
     </row>
     <row r="40" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A40" s="13" t="str">
+      <c r="A40" s="11" t="str">
         <f>[2]Sheet1!$A39</f>
         <v>MMS18-20/038</v>
       </c>
@@ -30477,7 +30314,7 @@
       </c>
       <c r="E40" s="6" t="str">
         <f>'[3]Subject Marks'!$T40</f>
-        <v>A</v>
+        <v>B+</v>
       </c>
       <c r="F40" s="6" t="str">
         <f>'[3]Subject Marks'!$AA40</f>
@@ -30509,7 +30346,7 @@
       </c>
     </row>
     <row r="41" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A41" s="13" t="str">
+      <c r="A41" s="11" t="str">
         <f>[2]Sheet1!$A40</f>
         <v>MMS18-20/039</v>
       </c>
@@ -30527,7 +30364,7 @@
       </c>
       <c r="E41" s="6" t="str">
         <f>'[3]Subject Marks'!$T41</f>
-        <v>A+</v>
+        <v>A</v>
       </c>
       <c r="F41" s="6" t="str">
         <f>'[3]Subject Marks'!$AA41</f>
@@ -30559,7 +30396,7 @@
       </c>
     </row>
     <row r="42" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A42" s="13" t="str">
+      <c r="A42" s="11" t="str">
         <f>[2]Sheet1!$A41</f>
         <v>MMS18-20/040</v>
       </c>
@@ -30577,7 +30414,7 @@
       </c>
       <c r="E42" s="6" t="str">
         <f>'[3]Subject Marks'!$T42</f>
-        <v>A+</v>
+        <v>A</v>
       </c>
       <c r="F42" s="6" t="str">
         <f>'[3]Subject Marks'!$AA42</f>
@@ -30609,7 +30446,7 @@
       </c>
     </row>
     <row r="43" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A43" s="13" t="str">
+      <c r="A43" s="11" t="str">
         <f>[2]Sheet1!$A42</f>
         <v>MMS18-20/041</v>
       </c>
@@ -30659,7 +30496,7 @@
       </c>
     </row>
     <row r="44" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A44" s="13" t="str">
+      <c r="A44" s="11" t="str">
         <f>[2]Sheet1!$A43</f>
         <v>MMS18-20/042</v>
       </c>
@@ -30677,7 +30514,7 @@
       </c>
       <c r="E44" s="6" t="str">
         <f>'[3]Subject Marks'!$T44</f>
-        <v>A</v>
+        <v>B+</v>
       </c>
       <c r="F44" s="6" t="str">
         <f>'[3]Subject Marks'!$AA44</f>
@@ -30709,7 +30546,7 @@
       </c>
     </row>
     <row r="45" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A45" s="13" t="str">
+      <c r="A45" s="11" t="str">
         <f>[2]Sheet1!$A44</f>
         <v>MMS18-20/043</v>
       </c>
@@ -30759,7 +30596,7 @@
       </c>
     </row>
     <row r="46" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A46" s="13" t="str">
+      <c r="A46" s="11" t="str">
         <f>[2]Sheet1!$A45</f>
         <v>MMS18-20/044</v>
       </c>
@@ -30777,7 +30614,7 @@
       </c>
       <c r="E46" s="6" t="str">
         <f>'[3]Subject Marks'!$T46</f>
-        <v>A</v>
+        <v>B+</v>
       </c>
       <c r="F46" s="6" t="str">
         <f>'[3]Subject Marks'!$AA46</f>
@@ -30809,7 +30646,7 @@
       </c>
     </row>
     <row r="47" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A47" s="13" t="str">
+      <c r="A47" s="11" t="str">
         <f>[2]Sheet1!$A46</f>
         <v>MMS18-20/045</v>
       </c>
@@ -30827,7 +30664,7 @@
       </c>
       <c r="E47" s="6" t="str">
         <f>'[3]Subject Marks'!$T47</f>
-        <v>A+</v>
+        <v>A</v>
       </c>
       <c r="F47" s="6" t="str">
         <f>'[3]Subject Marks'!$AA47</f>
@@ -30859,7 +30696,7 @@
       </c>
     </row>
     <row r="48" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A48" s="13" t="str">
+      <c r="A48" s="11" t="str">
         <f>[2]Sheet1!$A47</f>
         <v>MMS18-20/046</v>
       </c>
@@ -30877,7 +30714,7 @@
       </c>
       <c r="E48" s="6" t="str">
         <f>'[3]Subject Marks'!$T48</f>
-        <v>A</v>
+        <v>B</v>
       </c>
       <c r="F48" s="6" t="str">
         <f>'[3]Subject Marks'!$AA48</f>
@@ -30909,7 +30746,7 @@
       </c>
     </row>
     <row r="49" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A49" s="13" t="str">
+      <c r="A49" s="11" t="str">
         <f>[2]Sheet1!$A48</f>
         <v>MMS18-20/047</v>
       </c>
@@ -30927,7 +30764,7 @@
       </c>
       <c r="E49" s="6" t="str">
         <f>'[3]Subject Marks'!$T49</f>
-        <v>A+</v>
+        <v>A</v>
       </c>
       <c r="F49" s="6" t="str">
         <f>'[3]Subject Marks'!$AA49</f>
@@ -30959,7 +30796,7 @@
       </c>
     </row>
     <row r="50" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A50" s="13" t="str">
+      <c r="A50" s="11" t="str">
         <f>[2]Sheet1!$A49</f>
         <v>MMS18-20/048</v>
       </c>
@@ -31009,7 +30846,7 @@
       </c>
     </row>
     <row r="51" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A51" s="13" t="str">
+      <c r="A51" s="11" t="str">
         <f>[2]Sheet1!$A50</f>
         <v>MMS18-20/049</v>
       </c>
@@ -31027,7 +30864,7 @@
       </c>
       <c r="E51" s="6" t="str">
         <f>'[3]Subject Marks'!$T51</f>
-        <v>A</v>
+        <v>B+</v>
       </c>
       <c r="F51" s="6" t="str">
         <f>'[3]Subject Marks'!$AA51</f>
@@ -31059,7 +30896,7 @@
       </c>
     </row>
     <row r="52" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A52" s="13" t="str">
+      <c r="A52" s="11" t="str">
         <f>[2]Sheet1!$A51</f>
         <v>MMS18-20/050</v>
       </c>
@@ -31077,7 +30914,7 @@
       </c>
       <c r="E52" s="6" t="str">
         <f>'[3]Subject Marks'!$T52</f>
-        <v>A+</v>
+        <v>A</v>
       </c>
       <c r="F52" s="6" t="str">
         <f>'[3]Subject Marks'!$AA52</f>
@@ -31109,7 +30946,7 @@
       </c>
     </row>
     <row r="53" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A53" s="13" t="str">
+      <c r="A53" s="11" t="str">
         <f>[2]Sheet1!$A52</f>
         <v>MMS18-20/051</v>
       </c>
@@ -31127,7 +30964,7 @@
       </c>
       <c r="E53" s="6" t="str">
         <f>'[3]Subject Marks'!$T53</f>
-        <v>A+</v>
+        <v>A</v>
       </c>
       <c r="F53" s="6" t="str">
         <f>'[3]Subject Marks'!$AA53</f>
@@ -31159,7 +30996,7 @@
       </c>
     </row>
     <row r="54" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A54" s="13" t="str">
+      <c r="A54" s="11" t="str">
         <f>[2]Sheet1!$A53</f>
         <v>MMS18-20/052</v>
       </c>
@@ -31209,7 +31046,7 @@
       </c>
     </row>
     <row r="55" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A55" s="13" t="str">
+      <c r="A55" s="11" t="str">
         <f>[2]Sheet1!$A54</f>
         <v>MMS18-20/053</v>
       </c>
@@ -31227,7 +31064,7 @@
       </c>
       <c r="E55" s="6" t="str">
         <f>'[3]Subject Marks'!$T55</f>
-        <v>A</v>
+        <v>B+</v>
       </c>
       <c r="F55" s="6" t="str">
         <f>'[3]Subject Marks'!$AA55</f>
@@ -31259,7 +31096,7 @@
       </c>
     </row>
     <row r="56" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A56" s="13" t="str">
+      <c r="A56" s="11" t="str">
         <f>[2]Sheet1!$A55</f>
         <v>MMS18-20/054</v>
       </c>
@@ -31277,7 +31114,7 @@
       </c>
       <c r="E56" s="6" t="str">
         <f>'[3]Subject Marks'!$T56</f>
-        <v>A</v>
+        <v>B+</v>
       </c>
       <c r="F56" s="6" t="str">
         <f>'[3]Subject Marks'!$AA56</f>
@@ -31309,7 +31146,7 @@
       </c>
     </row>
     <row r="57" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A57" s="13" t="str">
+      <c r="A57" s="11" t="str">
         <f>[2]Sheet1!$A56</f>
         <v>MMS18-20/055</v>
       </c>
@@ -31327,7 +31164,7 @@
       </c>
       <c r="E57" s="6" t="str">
         <f>'[3]Subject Marks'!$T57</f>
-        <v>A</v>
+        <v>B+</v>
       </c>
       <c r="F57" s="6" t="str">
         <f>'[3]Subject Marks'!$AA57</f>
@@ -31359,7 +31196,7 @@
       </c>
     </row>
     <row r="58" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A58" s="13" t="str">
+      <c r="A58" s="11" t="str">
         <f>[2]Sheet1!$A57</f>
         <v>MMS18-20/056</v>
       </c>
@@ -31377,7 +31214,7 @@
       </c>
       <c r="E58" s="6" t="str">
         <f>'[3]Subject Marks'!$T58</f>
-        <v>A+</v>
+        <v>A</v>
       </c>
       <c r="F58" s="6" t="str">
         <f>'[3]Subject Marks'!$AA58</f>
@@ -31409,7 +31246,7 @@
       </c>
     </row>
     <row r="59" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A59" s="13" t="str">
+      <c r="A59" s="11" t="str">
         <f>[2]Sheet1!$A58</f>
         <v>MMS18-20/057</v>
       </c>
@@ -31427,7 +31264,7 @@
       </c>
       <c r="E59" s="6" t="str">
         <f>'[3]Subject Marks'!$T59</f>
-        <v>A</v>
+        <v>B</v>
       </c>
       <c r="F59" s="6" t="str">
         <f>'[3]Subject Marks'!$AA59</f>
@@ -31459,7 +31296,7 @@
       </c>
     </row>
     <row r="60" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A60" s="13" t="str">
+      <c r="A60" s="11" t="str">
         <f>[2]Sheet1!$A59</f>
         <v>MMS18-20/058</v>
       </c>
@@ -31477,7 +31314,7 @@
       </c>
       <c r="E60" s="6" t="str">
         <f>'[3]Subject Marks'!$T60</f>
-        <v>A+</v>
+        <v>A</v>
       </c>
       <c r="F60" s="6" t="str">
         <f>'[3]Subject Marks'!$AA60</f>
@@ -31509,7 +31346,7 @@
       </c>
     </row>
     <row r="61" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A61" s="13" t="str">
+      <c r="A61" s="11" t="str">
         <f>[2]Sheet1!$A60</f>
         <v>MMS18-20/059</v>
       </c>
@@ -31559,7 +31396,7 @@
       </c>
     </row>
     <row r="62" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A62" s="13" t="str">
+      <c r="A62" s="11" t="str">
         <f>[2]Sheet1!$A61</f>
         <v>MMS18-20/060</v>
       </c>
@@ -31577,7 +31414,7 @@
       </c>
       <c r="E62" s="6" t="str">
         <f>'[3]Subject Marks'!$T62</f>
-        <v>A</v>
+        <v>B+</v>
       </c>
       <c r="F62" s="6" t="str">
         <f>'[3]Subject Marks'!$AA62</f>
@@ -31609,7 +31446,7 @@
       </c>
     </row>
     <row r="63" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A63" s="13" t="str">
+      <c r="A63" s="11" t="str">
         <f>[2]Sheet1!$A62</f>
         <v>MMS18-20/061</v>
       </c>
@@ -31627,7 +31464,7 @@
       </c>
       <c r="E63" s="6" t="str">
         <f>'[3]Subject Marks'!$T63</f>
-        <v>A+</v>
+        <v>A</v>
       </c>
       <c r="F63" s="6" t="str">
         <f>'[3]Subject Marks'!$AA63</f>
@@ -31659,7 +31496,7 @@
       </c>
     </row>
     <row r="64" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A64" s="13" t="str">
+      <c r="A64" s="11" t="str">
         <f>[2]Sheet1!$A63</f>
         <v>MMS18-20/062</v>
       </c>
@@ -31677,7 +31514,7 @@
       </c>
       <c r="E64" s="6" t="str">
         <f>'[3]Subject Marks'!$T64</f>
-        <v>A+</v>
+        <v>A</v>
       </c>
       <c r="F64" s="6" t="str">
         <f>'[3]Subject Marks'!$AA64</f>
@@ -31709,7 +31546,7 @@
       </c>
     </row>
     <row r="65" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A65" s="13" t="str">
+      <c r="A65" s="11" t="str">
         <f>[2]Sheet1!$A64</f>
         <v>MMS18-20/063</v>
       </c>
@@ -31759,7 +31596,7 @@
       </c>
     </row>
     <row r="66" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A66" s="13" t="str">
+      <c r="A66" s="11" t="str">
         <f>[2]Sheet1!$A65</f>
         <v>MMS18-20/064</v>
       </c>
@@ -31777,7 +31614,7 @@
       </c>
       <c r="E66" s="6" t="str">
         <f>'[3]Subject Marks'!$T66</f>
-        <v>A</v>
+        <v>B+</v>
       </c>
       <c r="F66" s="6" t="str">
         <f>'[3]Subject Marks'!$AA66</f>
@@ -31809,7 +31646,7 @@
       </c>
     </row>
     <row r="67" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A67" s="13" t="str">
+      <c r="A67" s="11" t="str">
         <f>[2]Sheet1!$A66</f>
         <v>MMS18-20/065</v>
       </c>
@@ -31827,7 +31664,7 @@
       </c>
       <c r="E67" s="6" t="str">
         <f>'[3]Subject Marks'!$T67</f>
-        <v>A</v>
+        <v>B+</v>
       </c>
       <c r="F67" s="6" t="str">
         <f>'[3]Subject Marks'!$AA67</f>
@@ -31859,7 +31696,7 @@
       </c>
     </row>
     <row r="68" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A68" s="13" t="str">
+      <c r="A68" s="11" t="str">
         <f>[2]Sheet1!$A67</f>
         <v>MMS18-20/066</v>
       </c>
@@ -31877,7 +31714,7 @@
       </c>
       <c r="E68" s="6" t="str">
         <f>'[3]Subject Marks'!$T68</f>
-        <v>A</v>
+        <v>B+</v>
       </c>
       <c r="F68" s="6" t="str">
         <f>'[3]Subject Marks'!$AA68</f>
@@ -31909,7 +31746,7 @@
       </c>
     </row>
     <row r="69" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A69" s="13" t="str">
+      <c r="A69" s="11" t="str">
         <f>[2]Sheet1!$A68</f>
         <v>MMS18-20/067</v>
       </c>
@@ -31927,7 +31764,7 @@
       </c>
       <c r="E69" s="6" t="str">
         <f>'[3]Subject Marks'!$T69</f>
-        <v>A+</v>
+        <v>A</v>
       </c>
       <c r="F69" s="6" t="str">
         <f>'[3]Subject Marks'!$AA69</f>
@@ -31959,7 +31796,7 @@
       </c>
     </row>
     <row r="70" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A70" s="13" t="str">
+      <c r="A70" s="11" t="str">
         <f>[2]Sheet1!$A69</f>
         <v>MMS18-20/068</v>
       </c>
@@ -31977,7 +31814,7 @@
       </c>
       <c r="E70" s="6" t="str">
         <f>'[3]Subject Marks'!$T70</f>
-        <v>A</v>
+        <v>B</v>
       </c>
       <c r="F70" s="6" t="str">
         <f>'[3]Subject Marks'!$AA70</f>
@@ -32009,7 +31846,7 @@
       </c>
     </row>
     <row r="71" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A71" s="13" t="str">
+      <c r="A71" s="11" t="str">
         <f>[2]Sheet1!$A70</f>
         <v>MMS18-20/069</v>
       </c>
@@ -32027,7 +31864,7 @@
       </c>
       <c r="E71" s="6" t="str">
         <f>'[3]Subject Marks'!$T71</f>
-        <v>A+</v>
+        <v>A</v>
       </c>
       <c r="F71" s="6" t="str">
         <f>'[3]Subject Marks'!$AA71</f>
@@ -32059,7 +31896,7 @@
       </c>
     </row>
     <row r="72" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A72" s="13" t="str">
+      <c r="A72" s="11" t="str">
         <f>[2]Sheet1!$A71</f>
         <v>MMS18-20/070</v>
       </c>
@@ -32109,7 +31946,7 @@
       </c>
     </row>
     <row r="73" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A73" s="13" t="str">
+      <c r="A73" s="11" t="str">
         <f>[2]Sheet1!$A72</f>
         <v>MMS18-20/071</v>
       </c>
@@ -32127,7 +31964,7 @@
       </c>
       <c r="E73" s="6" t="str">
         <f>'[3]Subject Marks'!$T73</f>
-        <v>A</v>
+        <v>B+</v>
       </c>
       <c r="F73" s="6" t="str">
         <f>'[3]Subject Marks'!$AA73</f>
@@ -32159,7 +31996,7 @@
       </c>
     </row>
     <row r="74" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A74" s="13" t="str">
+      <c r="A74" s="11" t="str">
         <f>[2]Sheet1!$A73</f>
         <v>MMS18-20/072</v>
       </c>
@@ -32177,7 +32014,7 @@
       </c>
       <c r="E74" s="6" t="str">
         <f>'[3]Subject Marks'!$T74</f>
-        <v>A+</v>
+        <v>A</v>
       </c>
       <c r="F74" s="6" t="str">
         <f>'[3]Subject Marks'!$AA74</f>
@@ -32209,7 +32046,7 @@
       </c>
     </row>
     <row r="75" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A75" s="13" t="str">
+      <c r="A75" s="11" t="str">
         <f>[2]Sheet1!$A74</f>
         <v>MMS18-20/073</v>
       </c>
@@ -32227,7 +32064,7 @@
       </c>
       <c r="E75" s="6" t="str">
         <f>'[3]Subject Marks'!$T75</f>
-        <v>A+</v>
+        <v>A</v>
       </c>
       <c r="F75" s="6" t="str">
         <f>'[3]Subject Marks'!$AA75</f>
@@ -32259,7 +32096,7 @@
       </c>
     </row>
     <row r="76" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A76" s="13" t="str">
+      <c r="A76" s="11" t="str">
         <f>[2]Sheet1!$A75</f>
         <v>MMS18-20/074</v>
       </c>
@@ -32309,7 +32146,7 @@
       </c>
     </row>
     <row r="77" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A77" s="13" t="str">
+      <c r="A77" s="11" t="str">
         <f>[2]Sheet1!$A76</f>
         <v>MMS18-20/075</v>
       </c>
@@ -32327,7 +32164,7 @@
       </c>
       <c r="E77" s="6" t="str">
         <f>'[3]Subject Marks'!$T77</f>
-        <v>A</v>
+        <v>B+</v>
       </c>
       <c r="F77" s="6" t="str">
         <f>'[3]Subject Marks'!$AA77</f>
@@ -32359,7 +32196,7 @@
       </c>
     </row>
     <row r="78" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A78" s="13" t="str">
+      <c r="A78" s="11" t="str">
         <f>[2]Sheet1!$A77</f>
         <v>MMS18-20/076</v>
       </c>
@@ -32377,7 +32214,7 @@
       </c>
       <c r="E78" s="6" t="str">
         <f>'[3]Subject Marks'!$T78</f>
-        <v>A</v>
+        <v>B+</v>
       </c>
       <c r="F78" s="6" t="str">
         <f>'[3]Subject Marks'!$AA78</f>
@@ -32409,7 +32246,7 @@
       </c>
     </row>
     <row r="79" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A79" s="13" t="str">
+      <c r="A79" s="11" t="str">
         <f>[2]Sheet1!$A78</f>
         <v>MMS18-20/077</v>
       </c>
@@ -32427,7 +32264,7 @@
       </c>
       <c r="E79" s="6" t="str">
         <f>'[3]Subject Marks'!$T79</f>
-        <v>A</v>
+        <v>B+</v>
       </c>
       <c r="F79" s="6" t="str">
         <f>'[3]Subject Marks'!$AA79</f>
@@ -32459,7 +32296,7 @@
       </c>
     </row>
     <row r="80" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A80" s="13" t="str">
+      <c r="A80" s="11" t="str">
         <f>[2]Sheet1!$A79</f>
         <v>MMS18-20/078</v>
       </c>
@@ -32477,7 +32314,7 @@
       </c>
       <c r="E80" s="6" t="str">
         <f>'[3]Subject Marks'!$T80</f>
-        <v>A+</v>
+        <v>A</v>
       </c>
       <c r="F80" s="6" t="str">
         <f>'[3]Subject Marks'!$AA80</f>
@@ -32509,7 +32346,7 @@
       </c>
     </row>
     <row r="81" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A81" s="13" t="str">
+      <c r="A81" s="11" t="str">
         <f>[2]Sheet1!$A80</f>
         <v>MMS18-20/079</v>
       </c>
@@ -32527,7 +32364,7 @@
       </c>
       <c r="E81" s="6" t="str">
         <f>'[3]Subject Marks'!$T81</f>
-        <v>A</v>
+        <v>B</v>
       </c>
       <c r="F81" s="6" t="str">
         <f>'[3]Subject Marks'!$AA81</f>
@@ -32559,7 +32396,7 @@
       </c>
     </row>
     <row r="82" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A82" s="13" t="str">
+      <c r="A82" s="11" t="str">
         <f>[2]Sheet1!$A81</f>
         <v>MMS18-20/080</v>
       </c>
@@ -32577,7 +32414,7 @@
       </c>
       <c r="E82" s="6" t="str">
         <f>'[3]Subject Marks'!$T82</f>
-        <v>A+</v>
+        <v>A</v>
       </c>
       <c r="F82" s="6" t="str">
         <f>'[3]Subject Marks'!$AA82</f>
@@ -32609,7 +32446,7 @@
       </c>
     </row>
     <row r="83" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A83" s="13" t="str">
+      <c r="A83" s="11" t="str">
         <f>[2]Sheet1!$A82</f>
         <v>MMS18-20/081</v>
       </c>
@@ -32659,7 +32496,7 @@
       </c>
     </row>
     <row r="84" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A84" s="13" t="str">
+      <c r="A84" s="11" t="str">
         <f>[2]Sheet1!$A83</f>
         <v>MMS18-20/082</v>
       </c>
@@ -32677,7 +32514,7 @@
       </c>
       <c r="E84" s="6" t="str">
         <f>'[3]Subject Marks'!$T84</f>
-        <v>A</v>
+        <v>B+</v>
       </c>
       <c r="F84" s="6" t="str">
         <f>'[3]Subject Marks'!$AA84</f>
@@ -32709,7 +32546,7 @@
       </c>
     </row>
     <row r="85" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A85" s="13" t="str">
+      <c r="A85" s="11" t="str">
         <f>[2]Sheet1!$A84</f>
         <v>MMS18-20/083</v>
       </c>
@@ -32727,7 +32564,7 @@
       </c>
       <c r="E85" s="6" t="str">
         <f>'[3]Subject Marks'!$T85</f>
-        <v>A+</v>
+        <v>A</v>
       </c>
       <c r="F85" s="6" t="str">
         <f>'[3]Subject Marks'!$AA85</f>
@@ -32759,7 +32596,7 @@
       </c>
     </row>
     <row r="86" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A86" s="13" t="str">
+      <c r="A86" s="11" t="str">
         <f>[2]Sheet1!$A85</f>
         <v>MMS18-20/084</v>
       </c>
@@ -32777,7 +32614,7 @@
       </c>
       <c r="E86" s="6" t="str">
         <f>'[3]Subject Marks'!$T86</f>
-        <v>A+</v>
+        <v>A</v>
       </c>
       <c r="F86" s="6" t="str">
         <f>'[3]Subject Marks'!$AA86</f>
@@ -32809,7 +32646,7 @@
       </c>
     </row>
     <row r="87" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A87" s="13" t="str">
+      <c r="A87" s="11" t="str">
         <f>[2]Sheet1!$A86</f>
         <v>MMS18-20/085</v>
       </c>
@@ -32859,7 +32696,7 @@
       </c>
     </row>
     <row r="88" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A88" s="13" t="str">
+      <c r="A88" s="11" t="str">
         <f>[2]Sheet1!$A87</f>
         <v>MMS18-20/086</v>
       </c>
@@ -32877,7 +32714,7 @@
       </c>
       <c r="E88" s="6" t="str">
         <f>'[3]Subject Marks'!$T88</f>
-        <v>A</v>
+        <v>B+</v>
       </c>
       <c r="F88" s="6" t="str">
         <f>'[3]Subject Marks'!$AA88</f>
@@ -32909,7 +32746,7 @@
       </c>
     </row>
     <row r="89" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A89" s="13" t="str">
+      <c r="A89" s="11" t="str">
         <f>[2]Sheet1!$A88</f>
         <v>MMS18-20/087</v>
       </c>
@@ -32927,7 +32764,7 @@
       </c>
       <c r="E89" s="6" t="str">
         <f>'[3]Subject Marks'!$T89</f>
-        <v>A</v>
+        <v>B+</v>
       </c>
       <c r="F89" s="6" t="str">
         <f>'[3]Subject Marks'!$AA89</f>
@@ -32959,7 +32796,7 @@
       </c>
     </row>
     <row r="90" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A90" s="13" t="str">
+      <c r="A90" s="11" t="str">
         <f>[2]Sheet1!$A89</f>
         <v>MMS18-20/088</v>
       </c>
@@ -32977,7 +32814,7 @@
       </c>
       <c r="E90" s="6" t="str">
         <f>'[3]Subject Marks'!$T90</f>
-        <v>A</v>
+        <v>B+</v>
       </c>
       <c r="F90" s="6" t="str">
         <f>'[3]Subject Marks'!$AA90</f>
@@ -33009,7 +32846,7 @@
       </c>
     </row>
     <row r="91" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A91" s="13" t="str">
+      <c r="A91" s="11" t="str">
         <f>[2]Sheet1!$A90</f>
         <v>MMS18-20/089</v>
       </c>
@@ -33027,7 +32864,7 @@
       </c>
       <c r="E91" s="6" t="str">
         <f>'[3]Subject Marks'!$T91</f>
-        <v>A+</v>
+        <v>A</v>
       </c>
       <c r="F91" s="6" t="str">
         <f>'[3]Subject Marks'!$AA91</f>
@@ -33059,7 +32896,7 @@
       </c>
     </row>
     <row r="92" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A92" s="13" t="str">
+      <c r="A92" s="11" t="str">
         <f>[2]Sheet1!$A91</f>
         <v>MMS18-20/090</v>
       </c>
@@ -33077,7 +32914,7 @@
       </c>
       <c r="E92" s="6" t="str">
         <f>'[3]Subject Marks'!$T92</f>
-        <v>A</v>
+        <v>B</v>
       </c>
       <c r="F92" s="6" t="str">
         <f>'[3]Subject Marks'!$AA92</f>
@@ -33109,7 +32946,7 @@
       </c>
     </row>
     <row r="93" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A93" s="13" t="str">
+      <c r="A93" s="11" t="str">
         <f>[2]Sheet1!$A92</f>
         <v>MMS18-20/091</v>
       </c>
@@ -33127,7 +32964,7 @@
       </c>
       <c r="E93" s="6" t="str">
         <f>'[3]Subject Marks'!$T93</f>
-        <v>A+</v>
+        <v>A</v>
       </c>
       <c r="F93" s="6" t="str">
         <f>'[3]Subject Marks'!$AA93</f>
@@ -33159,7 +32996,7 @@
       </c>
     </row>
     <row r="94" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A94" s="13" t="str">
+      <c r="A94" s="11" t="str">
         <f>[2]Sheet1!$A93</f>
         <v>MMS18-20/092</v>
       </c>
@@ -33209,7 +33046,7 @@
       </c>
     </row>
     <row r="95" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A95" s="13" t="str">
+      <c r="A95" s="11" t="str">
         <f>[2]Sheet1!$A94</f>
         <v>MMS18-20/093</v>
       </c>
@@ -33227,7 +33064,7 @@
       </c>
       <c r="E95" s="6" t="str">
         <f>'[3]Subject Marks'!$T95</f>
-        <v>A</v>
+        <v>B+</v>
       </c>
       <c r="F95" s="6" t="str">
         <f>'[3]Subject Marks'!$AA95</f>
@@ -33259,7 +33096,7 @@
       </c>
     </row>
     <row r="96" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A96" s="13" t="str">
+      <c r="A96" s="11" t="str">
         <f>[2]Sheet1!$A95</f>
         <v>MMS18-20/094</v>
       </c>
@@ -33277,7 +33114,7 @@
       </c>
       <c r="E96" s="6" t="str">
         <f>'[3]Subject Marks'!$T96</f>
-        <v>A+</v>
+        <v>A</v>
       </c>
       <c r="F96" s="6" t="str">
         <f>'[3]Subject Marks'!$AA96</f>
@@ -33309,7 +33146,7 @@
       </c>
     </row>
     <row r="97" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A97" s="13" t="str">
+      <c r="A97" s="11" t="str">
         <f>[2]Sheet1!$A96</f>
         <v>MMS18-20/095</v>
       </c>
@@ -33327,7 +33164,7 @@
       </c>
       <c r="E97" s="6" t="str">
         <f>'[3]Subject Marks'!$T97</f>
-        <v>A+</v>
+        <v>A</v>
       </c>
       <c r="F97" s="6" t="str">
         <f>'[3]Subject Marks'!$AA97</f>
@@ -33359,7 +33196,7 @@
       </c>
     </row>
     <row r="98" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A98" s="13" t="str">
+      <c r="A98" s="11" t="str">
         <f>[2]Sheet1!$A97</f>
         <v>MMS18-20/096</v>
       </c>
@@ -33409,7 +33246,7 @@
       </c>
     </row>
     <row r="99" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A99" s="13" t="str">
+      <c r="A99" s="11" t="str">
         <f>[2]Sheet1!$A98</f>
         <v>MMS18-20/097</v>
       </c>
@@ -33427,7 +33264,7 @@
       </c>
       <c r="E99" s="6" t="str">
         <f>'[3]Subject Marks'!$T99</f>
-        <v>A</v>
+        <v>B+</v>
       </c>
       <c r="F99" s="6" t="str">
         <f>'[3]Subject Marks'!$AA99</f>
@@ -33459,7 +33296,7 @@
       </c>
     </row>
     <row r="100" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A100" s="13" t="str">
+      <c r="A100" s="11" t="str">
         <f>[2]Sheet1!$A99</f>
         <v>MMS18-20/098</v>
       </c>
@@ -33477,7 +33314,7 @@
       </c>
       <c r="E100" s="6" t="str">
         <f>'[3]Subject Marks'!$T100</f>
-        <v>A</v>
+        <v>B+</v>
       </c>
       <c r="F100" s="6" t="str">
         <f>'[3]Subject Marks'!$AA100</f>
@@ -33509,7 +33346,7 @@
       </c>
     </row>
     <row r="101" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A101" s="13" t="str">
+      <c r="A101" s="11" t="str">
         <f>[2]Sheet1!$A100</f>
         <v>MMS18-20/099</v>
       </c>
@@ -33527,7 +33364,7 @@
       </c>
       <c r="E101" s="6" t="str">
         <f>'[3]Subject Marks'!$T101</f>
-        <v>A</v>
+        <v>B+</v>
       </c>
       <c r="F101" s="6" t="str">
         <f>'[3]Subject Marks'!$AA101</f>
@@ -33559,7 +33396,7 @@
       </c>
     </row>
     <row r="102" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A102" s="13" t="str">
+      <c r="A102" s="11" t="str">
         <f>[2]Sheet1!$A101</f>
         <v>MMS18-20/100</v>
       </c>
@@ -33577,7 +33414,7 @@
       </c>
       <c r="E102" s="6" t="str">
         <f>'[3]Subject Marks'!$T102</f>
-        <v>A+</v>
+        <v>A</v>
       </c>
       <c r="F102" s="6" t="str">
         <f>'[3]Subject Marks'!$AA102</f>
@@ -33609,7 +33446,7 @@
       </c>
     </row>
     <row r="103" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A103" s="13" t="str">
+      <c r="A103" s="11" t="str">
         <f>[2]Sheet1!$A102</f>
         <v>MMS18-20/101</v>
       </c>
@@ -33627,7 +33464,7 @@
       </c>
       <c r="E103" s="6" t="str">
         <f>'[3]Subject Marks'!$T103</f>
-        <v>A</v>
+        <v>B</v>
       </c>
       <c r="F103" s="6" t="str">
         <f>'[3]Subject Marks'!$AA103</f>
@@ -33659,7 +33496,7 @@
       </c>
     </row>
     <row r="104" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A104" s="13" t="str">
+      <c r="A104" s="11" t="str">
         <f>[2]Sheet1!$A103</f>
         <v>MMS18-20/102</v>
       </c>
@@ -33677,7 +33514,7 @@
       </c>
       <c r="E104" s="6" t="str">
         <f>'[3]Subject Marks'!$T104</f>
-        <v>A+</v>
+        <v>A</v>
       </c>
       <c r="F104" s="6" t="str">
         <f>'[3]Subject Marks'!$AA104</f>
@@ -33709,7 +33546,7 @@
       </c>
     </row>
     <row r="105" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A105" s="13" t="str">
+      <c r="A105" s="11" t="str">
         <f>[2]Sheet1!$A104</f>
         <v>MMS18-20/103</v>
       </c>
@@ -33759,7 +33596,7 @@
       </c>
     </row>
     <row r="106" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A106" s="13" t="str">
+      <c r="A106" s="11" t="str">
         <f>[2]Sheet1!$A105</f>
         <v>MMS18-20/104</v>
       </c>
@@ -33777,7 +33614,7 @@
       </c>
       <c r="E106" s="6" t="str">
         <f>'[3]Subject Marks'!$T106</f>
-        <v>A</v>
+        <v>B+</v>
       </c>
       <c r="F106" s="6" t="str">
         <f>'[3]Subject Marks'!$AA106</f>
@@ -33809,7 +33646,7 @@
       </c>
     </row>
     <row r="107" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A107" s="13" t="str">
+      <c r="A107" s="11" t="str">
         <f>[2]Sheet1!$A106</f>
         <v>MMS18-20/105</v>
       </c>
@@ -33827,7 +33664,7 @@
       </c>
       <c r="E107" s="6" t="str">
         <f>'[3]Subject Marks'!$T107</f>
-        <v>A+</v>
+        <v>A</v>
       </c>
       <c r="F107" s="6" t="str">
         <f>'[3]Subject Marks'!$AA107</f>
@@ -33859,7 +33696,7 @@
       </c>
     </row>
     <row r="108" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A108" s="13" t="str">
+      <c r="A108" s="11" t="str">
         <f>[2]Sheet1!$A107</f>
         <v>MMS18-20/106</v>
       </c>
@@ -33877,7 +33714,7 @@
       </c>
       <c r="E108" s="6" t="str">
         <f>'[3]Subject Marks'!$T108</f>
-        <v>A+</v>
+        <v>A</v>
       </c>
       <c r="F108" s="6" t="str">
         <f>'[3]Subject Marks'!$AA108</f>
@@ -33909,7 +33746,7 @@
       </c>
     </row>
     <row r="109" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A109" s="13" t="str">
+      <c r="A109" s="11" t="str">
         <f>[2]Sheet1!$A108</f>
         <v>MMS18-20/107</v>
       </c>
@@ -33959,7 +33796,7 @@
       </c>
     </row>
     <row r="110" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A110" s="13" t="str">
+      <c r="A110" s="11" t="str">
         <f>[2]Sheet1!$A109</f>
         <v>MMS18-20/108</v>
       </c>
@@ -33977,7 +33814,7 @@
       </c>
       <c r="E110" s="6" t="str">
         <f>'[3]Subject Marks'!$T110</f>
-        <v>A</v>
+        <v>B+</v>
       </c>
       <c r="F110" s="6" t="str">
         <f>'[3]Subject Marks'!$AA110</f>
@@ -34009,7 +33846,7 @@
       </c>
     </row>
     <row r="111" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A111" s="13" t="str">
+      <c r="A111" s="11" t="str">
         <f>[2]Sheet1!$A110</f>
         <v>MMS18-20/109</v>
       </c>
@@ -34027,7 +33864,7 @@
       </c>
       <c r="E111" s="6" t="str">
         <f>'[3]Subject Marks'!$T111</f>
-        <v>A</v>
+        <v>B+</v>
       </c>
       <c r="F111" s="6" t="str">
         <f>'[3]Subject Marks'!$AA111</f>
@@ -34059,7 +33896,7 @@
       </c>
     </row>
     <row r="112" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A112" s="13" t="str">
+      <c r="A112" s="11" t="str">
         <f>[2]Sheet1!$A111</f>
         <v>MMS18-20/110</v>
       </c>
@@ -34077,7 +33914,7 @@
       </c>
       <c r="E112" s="6" t="str">
         <f>'[3]Subject Marks'!$T112</f>
-        <v>A</v>
+        <v>B+</v>
       </c>
       <c r="F112" s="6" t="str">
         <f>'[3]Subject Marks'!$AA112</f>
@@ -34109,7 +33946,7 @@
       </c>
     </row>
     <row r="113" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A113" s="13" t="str">
+      <c r="A113" s="11" t="str">
         <f>[2]Sheet1!$A112</f>
         <v>MMS18-20/111</v>
       </c>
@@ -34127,7 +33964,7 @@
       </c>
       <c r="E113" s="6" t="str">
         <f>'[3]Subject Marks'!$T113</f>
-        <v>A+</v>
+        <v>A</v>
       </c>
       <c r="F113" s="6" t="str">
         <f>'[3]Subject Marks'!$AA113</f>
@@ -34159,7 +33996,7 @@
       </c>
     </row>
     <row r="114" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A114" s="13" t="str">
+      <c r="A114" s="11" t="str">
         <f>[2]Sheet1!$A113</f>
         <v>MMS18-20/112</v>
       </c>
@@ -34177,7 +34014,7 @@
       </c>
       <c r="E114" s="6" t="str">
         <f>'[3]Subject Marks'!$T114</f>
-        <v>A</v>
+        <v>B</v>
       </c>
       <c r="F114" s="6" t="str">
         <f>'[3]Subject Marks'!$AA114</f>
@@ -34209,7 +34046,7 @@
       </c>
     </row>
     <row r="115" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A115" s="13" t="str">
+      <c r="A115" s="11" t="str">
         <f>[2]Sheet1!$A114</f>
         <v>MMS18-20/113</v>
       </c>
@@ -34227,7 +34064,7 @@
       </c>
       <c r="E115" s="6" t="str">
         <f>'[3]Subject Marks'!$T115</f>
-        <v>A+</v>
+        <v>A</v>
       </c>
       <c r="F115" s="6" t="str">
         <f>'[3]Subject Marks'!$AA115</f>
@@ -34259,7 +34096,7 @@
       </c>
     </row>
     <row r="116" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A116" s="13" t="str">
+      <c r="A116" s="11" t="str">
         <f>[2]Sheet1!$A115</f>
         <v>MMS18-20/114</v>
       </c>
@@ -34309,7 +34146,7 @@
       </c>
     </row>
     <row r="117" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A117" s="13" t="str">
+      <c r="A117" s="11" t="str">
         <f>[2]Sheet1!$A116</f>
         <v>MMS18-20/115</v>
       </c>
@@ -34327,7 +34164,7 @@
       </c>
       <c r="E117" s="6" t="str">
         <f>'[3]Subject Marks'!$T117</f>
-        <v>A</v>
+        <v>B+</v>
       </c>
       <c r="F117" s="6" t="str">
         <f>'[3]Subject Marks'!$AA117</f>
@@ -34359,7 +34196,7 @@
       </c>
     </row>
     <row r="118" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A118" s="13" t="str">
+      <c r="A118" s="11" t="str">
         <f>[2]Sheet1!$A117</f>
         <v>MMS18-20/116</v>
       </c>
@@ -34377,7 +34214,7 @@
       </c>
       <c r="E118" s="6" t="str">
         <f>'[3]Subject Marks'!$T118</f>
-        <v>A+</v>
+        <v>A</v>
       </c>
       <c r="F118" s="6" t="str">
         <f>'[3]Subject Marks'!$AA118</f>
@@ -34409,7 +34246,7 @@
       </c>
     </row>
     <row r="119" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A119" s="13" t="str">
+      <c r="A119" s="11" t="str">
         <f>[2]Sheet1!$A118</f>
         <v>MMS18-20/117</v>
       </c>
@@ -34427,7 +34264,7 @@
       </c>
       <c r="E119" s="6" t="str">
         <f>'[3]Subject Marks'!$T119</f>
-        <v>A+</v>
+        <v>A</v>
       </c>
       <c r="F119" s="6" t="str">
         <f>'[3]Subject Marks'!$AA119</f>
@@ -34459,7 +34296,7 @@
       </c>
     </row>
     <row r="120" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A120" s="13" t="str">
+      <c r="A120" s="11" t="str">
         <f>[2]Sheet1!$A119</f>
         <v>MMS18-20/118</v>
       </c>
@@ -34509,7 +34346,7 @@
       </c>
     </row>
     <row r="121" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A121" s="13" t="str">
+      <c r="A121" s="11" t="str">
         <f>[2]Sheet1!$A120</f>
         <v>MMS18-20/119</v>
       </c>
@@ -34527,7 +34364,7 @@
       </c>
       <c r="E121" s="6" t="str">
         <f>'[3]Subject Marks'!$T121</f>
-        <v>A</v>
+        <v>B+</v>
       </c>
       <c r="F121" s="6" t="str">
         <f>'[3]Subject Marks'!$AA121</f>
@@ -34559,7 +34396,7 @@
       </c>
     </row>
     <row r="122" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A122" s="13" t="str">
+      <c r="A122" s="11" t="str">
         <f>[2]Sheet1!$A121</f>
         <v>MMS18-20/120</v>
       </c>
@@ -34609,7 +34446,7 @@
       </c>
     </row>
     <row r="123" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A123" s="13" t="str">
+      <c r="A123" s="11" t="str">
         <f>[2]Sheet1!$A122</f>
         <v>MMS18-20/121</v>
       </c>
@@ -34659,7 +34496,7 @@
       </c>
     </row>
     <row r="124" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A124" s="13" t="str">
+      <c r="A124" s="11" t="str">
         <f>[2]Sheet1!$A123</f>
         <v>MMS18-20/122</v>
       </c>
@@ -34709,7 +34546,7 @@
       </c>
     </row>
     <row r="125" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A125" s="13" t="str">
+      <c r="A125" s="11" t="str">
         <f>[2]Sheet1!$A124</f>
         <v>MMS18-20/123</v>
       </c>
@@ -34759,7 +34596,7 @@
       </c>
     </row>
     <row r="126" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A126" s="13" t="str">
+      <c r="A126" s="11" t="str">
         <f>[2]Sheet1!$A125</f>
         <v>MMS18-20/124</v>
       </c>
@@ -34809,7 +34646,7 @@
       </c>
     </row>
     <row r="127" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A127" s="13" t="str">
+      <c r="A127" s="11" t="str">
         <f>[2]Sheet1!$A126</f>
         <v>MMS18-20/125</v>
       </c>
@@ -34859,7 +34696,10 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="gC47o4LliIfIwcEYMknoJkkWrW0G3Ne+tO8DkSgrpykEwr8oYARNix0yOlsNck4sIYE7cE6TY8aOMh9vumgpGA==" saltValue="hHgIy7JXFbBux1xNIbdX/Q==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="MsCVtoa6hIEEzHf9L2e4NZxnr6b7TyzyFSjdQSDBms/BrItfSAqseVgwWK2Myls/IbpDz3JXXLSgClQGLDs9xA==" saltValue="ncC0a5FWJslR6YmpK9lGWg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <protectedRanges>
+    <protectedRange sqref="A128:L135" name="Blank Below"/>
+  </protectedRanges>
   <mergeCells count="2">
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="K1:L1"/>
@@ -34870,10 +34710,10 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L3:L127">
-    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="2" operator="equal">
       <formula>"F"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
       <formula>"F"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -34883,11 +34723,11 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3:J127">
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="lessThan">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+      <formula>"F"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="lessThan">
       <formula>51</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
-      <formula>"F"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3:K127">
@@ -34898,141 +34738,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C8CEBE1-20F9-4011-BEFB-AC3D9D6F5B6B}">
-  <dimension ref="A1:F16"/>
-  <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:F2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="6.7109375" style="27" customWidth="1"/>
-    <col min="2" max="2" width="10.7109375" style="29" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.42578125" style="29" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="85.140625" style="29" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.140625" style="29" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="27.42578125" style="29" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="29"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="2:6" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-    </row>
-    <row r="2" spans="2:6" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="24"/>
-    </row>
-    <row r="3" spans="2:6" ht="12" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B3" s="26"/>
-      <c r="C3" s="26"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="26"/>
-      <c r="F3" s="26"/>
-    </row>
-    <row r="4" spans="2:6" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="B4" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="D4" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="F4" s="14" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="2:6" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="B5" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="15"/>
-      <c r="D5" s="17"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="14"/>
-    </row>
-    <row r="6" spans="2:6" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="B6" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="15"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="14"/>
-    </row>
-    <row r="7" spans="2:6" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="B7" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" s="15"/>
-      <c r="D7" s="17"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="14"/>
-    </row>
-    <row r="8" spans="2:6" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="B8" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8" s="15"/>
-      <c r="D8" s="17"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14"/>
-    </row>
-    <row r="9" spans="2:6" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="B9" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="C9" s="15"/>
-      <c r="D9" s="17"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
-    </row>
-    <row r="10" spans="2:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="28"/>
-      <c r="C10" s="28"/>
-      <c r="D10" s="28"/>
-      <c r="E10" s="28"/>
-      <c r="F10" s="28"/>
-    </row>
-    <row r="11" spans="2:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="2:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="2:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="2:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="2:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="2:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.25"/>
-  </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="QBsVawiCh0BLwR6vyw8ArqghVGqveQ9hueHMnSfm+P6bRIS4fB85QmZIcoZTt9yLKALp7BaJijuLMYXVlt8kfA==" saltValue="P3JRr1me7uUYgkzxstLrug==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
-  <protectedRanges>
-    <protectedRange sqref="D15" name="RDO"/>
-    <protectedRange sqref="D13" name="HELD IN"/>
-    <protectedRange sqref="D4:D11" name="Subjects"/>
-  </protectedRanges>
-  <mergeCells count="6">
-    <mergeCell ref="G1:XFD1048576"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="B1:F1"/>
-    <mergeCell ref="B3:F3"/>
-    <mergeCell ref="A1:A1048576"/>
-    <mergeCell ref="B10:F1048576"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>